<commit_message>
Following adjustment. Survival analyses. Stage Early specification.
</commit_message>
<xml_diff>
--- a/output/tables/250428_partA_logistic_02.xlsx
+++ b/output/tables/250428_partA_logistic_02.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +402,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -411,28 +411,28 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.982</v>
+        <v>0.98</v>
       </c>
       <c r="D2">
-        <v>0.032</v>
+        <v>0.025</v>
       </c>
       <c r="E2">
-        <v>-0.5639999999999999</v>
+        <v>-0.789</v>
       </c>
       <c r="F2">
-        <v>0.573</v>
+        <v>0.43</v>
       </c>
       <c r="G2">
-        <v>0.923</v>
+        <v>0.929</v>
       </c>
       <c r="H2">
-        <v>1.05</v>
+        <v>1.028</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -441,28 +441,28 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.08</v>
+        <v>1.018</v>
       </c>
       <c r="D3">
-        <v>1.136</v>
+        <v>0.629</v>
       </c>
       <c r="E3">
-        <v>-2.224</v>
+        <v>0.029</v>
       </c>
       <c r="F3">
-        <v>0.026</v>
+        <v>0.977</v>
       </c>
       <c r="G3">
-        <v>0.004</v>
+        <v>0.29</v>
       </c>
       <c r="H3">
-        <v>0.539</v>
+        <v>3.503</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -471,28 +471,28 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.9320000000000001</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="D4">
-        <v>0.089</v>
+        <v>0.058</v>
       </c>
       <c r="E4">
-        <v>-0.798</v>
+        <v>-1.059</v>
       </c>
       <c r="F4">
-        <v>0.425</v>
+        <v>0.29</v>
       </c>
       <c r="G4">
-        <v>0.762</v>
+        <v>0.834</v>
       </c>
       <c r="H4">
-        <v>1.087</v>
+        <v>1.052</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -501,28 +501,28 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.308</v>
+        <v>1.011</v>
       </c>
       <c r="D5">
-        <v>1.134</v>
+        <v>0.679</v>
       </c>
       <c r="E5">
-        <v>-1.04</v>
+        <v>0.015</v>
       </c>
       <c r="F5">
-        <v>0.298</v>
+        <v>0.988</v>
       </c>
       <c r="G5">
-        <v>0.015</v>
+        <v>0.27</v>
       </c>
       <c r="H5">
-        <v>2.078</v>
+        <v>4.023</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -531,28 +531,28 @@
         </is>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>2.143</v>
       </c>
       <c r="D6">
-        <v>0.929</v>
+        <v>0.884</v>
       </c>
       <c r="E6">
-        <v>2.58</v>
+        <v>0.862</v>
       </c>
       <c r="F6">
-        <v>0.01</v>
+        <v>0.388</v>
       </c>
       <c r="G6">
-        <v>1.84</v>
+        <v>0.425</v>
       </c>
       <c r="H6">
-        <v>77.297</v>
+        <v>16.023</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -561,28 +561,28 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.34</v>
+        <v>1.786</v>
       </c>
       <c r="D7">
-        <v>0.899</v>
+        <v>0.627</v>
       </c>
       <c r="E7">
-        <v>-1.2</v>
+        <v>0.925</v>
       </c>
       <c r="F7">
-        <v>0.23</v>
+        <v>0.355</v>
       </c>
       <c r="G7">
-        <v>0.045</v>
+        <v>0.528</v>
       </c>
       <c r="H7">
-        <v>1.801</v>
+        <v>6.306</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>stage_early</t>
+          <t>response_achieved</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -591,231 +591,21 @@
         </is>
       </c>
       <c r="C8">
-        <v>14.182</v>
+        <v>1.65</v>
       </c>
       <c r="D8">
-        <v>1.138</v>
+        <v>0.661</v>
       </c>
       <c r="E8">
-        <v>2.329</v>
+        <v>0.758</v>
       </c>
       <c r="F8">
-        <v>0.02</v>
+        <v>0.449</v>
       </c>
       <c r="G8">
-        <v>2.093</v>
+        <v>0.464</v>
       </c>
       <c r="H8">
-        <v>285.022</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>0.98</v>
-      </c>
-      <c r="D9">
-        <v>0.025</v>
-      </c>
-      <c r="E9">
-        <v>-0.789</v>
-      </c>
-      <c r="F9">
-        <v>0.43</v>
-      </c>
-      <c r="G9">
-        <v>0.929</v>
-      </c>
-      <c r="H9">
-        <v>1.028</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>sex</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>1.018</v>
-      </c>
-      <c r="D10">
-        <v>0.629</v>
-      </c>
-      <c r="E10">
-        <v>0.029</v>
-      </c>
-      <c r="F10">
-        <v>0.977</v>
-      </c>
-      <c r="G10">
-        <v>0.29</v>
-      </c>
-      <c r="H10">
-        <v>3.503</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>bmi</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>0.9409999999999999</v>
-      </c>
-      <c r="D11">
-        <v>0.058</v>
-      </c>
-      <c r="E11">
-        <v>-1.059</v>
-      </c>
-      <c r="F11">
-        <v>0.29</v>
-      </c>
-      <c r="G11">
-        <v>0.834</v>
-      </c>
-      <c r="H11">
-        <v>1.052</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ps_ecog</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>1.011</v>
-      </c>
-      <c r="D12">
-        <v>0.679</v>
-      </c>
-      <c r="E12">
-        <v>0.015</v>
-      </c>
-      <c r="F12">
-        <v>0.988</v>
-      </c>
-      <c r="G12">
-        <v>0.27</v>
-      </c>
-      <c r="H12">
-        <v>4.023</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>first_syst_th</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>2.143</v>
-      </c>
-      <c r="D13">
-        <v>0.884</v>
-      </c>
-      <c r="E13">
-        <v>0.862</v>
-      </c>
-      <c r="F13">
-        <v>0.388</v>
-      </c>
-      <c r="G13">
-        <v>0.425</v>
-      </c>
-      <c r="H13">
-        <v>16.023</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ae_grade_3_4</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>1.786</v>
-      </c>
-      <c r="D14">
-        <v>0.627</v>
-      </c>
-      <c r="E14">
-        <v>0.925</v>
-      </c>
-      <c r="F14">
-        <v>0.355</v>
-      </c>
-      <c r="G14">
-        <v>0.528</v>
-      </c>
-      <c r="H14">
-        <v>6.306</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>response_achieved</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>monotherapy</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>1.65</v>
-      </c>
-      <c r="D15">
-        <v>0.661</v>
-      </c>
-      <c r="E15">
-        <v>0.758</v>
-      </c>
-      <c r="F15">
-        <v>0.449</v>
-      </c>
-      <c r="G15">
-        <v>0.464</v>
-      </c>
-      <c r="H15">
         <v>6.415</v>
       </c>
     </row>

</xml_diff>